<commit_message>
Assembler initiated. NOP, PSH, POP implemented. Opcodes Exel updated.
</commit_message>
<xml_diff>
--- a/opcodes-fic.xlsx
+++ b/opcodes-fic.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="136">
   <si>
     <t>Opcode</t>
   </si>
@@ -201,15 +201,9 @@
     <t>100001</t>
   </si>
   <si>
-    <t>ADDXY</t>
-  </si>
-  <si>
     <t>100010</t>
   </si>
   <si>
-    <t>ADDRA</t>
-  </si>
-  <si>
     <t>100011</t>
   </si>
   <si>
@@ -225,21 +219,12 @@
     <t>100101</t>
   </si>
   <si>
-    <t>SUBXY</t>
-  </si>
-  <si>
-    <t>SUBRA</t>
-  </si>
-  <si>
     <t>100110</t>
   </si>
   <si>
     <t>100111</t>
   </si>
   <si>
-    <t>Dxxxxxxxx</t>
-  </si>
-  <si>
     <t>SHIFT</t>
   </si>
   <si>
@@ -252,15 +237,9 @@
     <t>.</t>
   </si>
   <si>
-    <t>MUL</t>
-  </si>
-  <si>
     <t>101100</t>
   </si>
   <si>
-    <t>MULI</t>
-  </si>
-  <si>
     <t>101101</t>
   </si>
   <si>
@@ -270,30 +249,12 @@
     <t>101111</t>
   </si>
   <si>
-    <t>DIV</t>
-  </si>
-  <si>
-    <t>DIVI</t>
-  </si>
-  <si>
-    <t>MOD</t>
-  </si>
-  <si>
-    <t>MODI</t>
-  </si>
-  <si>
     <t>110000</t>
   </si>
   <si>
     <t>110001</t>
   </si>
   <si>
-    <t>AND</t>
-  </si>
-  <si>
-    <t>ANDI</t>
-  </si>
-  <si>
     <t>110010</t>
   </si>
   <si>
@@ -306,18 +267,6 @@
     <t>110101</t>
   </si>
   <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>ORI</t>
-  </si>
-  <si>
-    <t>XOR</t>
-  </si>
-  <si>
-    <t>XORI</t>
-  </si>
-  <si>
     <t>110110</t>
   </si>
   <si>
@@ -351,9 +300,6 @@
     <t>111001</t>
   </si>
   <si>
-    <t>CMP</t>
-  </si>
-  <si>
     <t>111110</t>
   </si>
   <si>
@@ -375,27 +321,12 @@
     <t>111111</t>
   </si>
   <si>
-    <t>CMPI</t>
-  </si>
-  <si>
     <t>CMPAI</t>
   </si>
   <si>
-    <t>SSDD xxxxxx</t>
-  </si>
-  <si>
-    <t>TSTI</t>
-  </si>
-  <si>
     <t>TSTAI</t>
   </si>
   <si>
-    <t>TST</t>
-  </si>
-  <si>
-    <t>SD xxxxxxxx</t>
-  </si>
-  <si>
     <t>001101</t>
   </si>
   <si>
@@ -418,13 +349,88 @@
   </si>
   <si>
     <t>CDD</t>
+  </si>
+  <si>
+    <t>MULAI</t>
+  </si>
+  <si>
+    <t>DIVAI</t>
+  </si>
+  <si>
+    <t>MODAI</t>
+  </si>
+  <si>
+    <t>CMPRI</t>
+  </si>
+  <si>
+    <t>CMPRR</t>
+  </si>
+  <si>
+    <t>TSTRI</t>
+  </si>
+  <si>
+    <t>TSTRR</t>
+  </si>
+  <si>
+    <t>ANDAI</t>
+  </si>
+  <si>
+    <t>ORAI</t>
+  </si>
+  <si>
+    <t>XORAI</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>X/Y/ACC/I</t>
+  </si>
+  <si>
+    <t>ACC^(X/Y/ACC/IMM)</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>Zero,Neg,Carry,Ovfl</t>
+  </si>
+  <si>
+    <t>!!</t>
+  </si>
+  <si>
+    <t>ADDRR</t>
+  </si>
+  <si>
+    <t>FFSSxxxxxx</t>
+  </si>
+  <si>
+    <t>SUBRR</t>
+  </si>
+  <si>
+    <t>MULRR</t>
+  </si>
+  <si>
+    <t>DIVRR</t>
+  </si>
+  <si>
+    <t>ANDRR</t>
+  </si>
+  <si>
+    <t>MODRR</t>
+  </si>
+  <si>
+    <t>ORRR</t>
+  </si>
+  <si>
+    <t>XORRR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -582,18 +588,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -602,7 +609,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,7 +704,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -727,7 +738,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -903,28 +913,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:F72"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65:F65"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="10.44140625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:7">
+      <c r="G2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7">
+      <c r="G3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -938,19 +960,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7">
       <c r="C6" s="2" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7">
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -964,7 +986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7">
       <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
@@ -978,7 +1000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7">
       <c r="C9" s="5" t="s">
         <v>54</v>
       </c>
@@ -992,7 +1014,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:7">
       <c r="C10" s="8" t="s">
         <v>55</v>
       </c>
@@ -1006,7 +1028,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7">
       <c r="C11" s="5" t="s">
         <v>46</v>
       </c>
@@ -1020,7 +1042,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7">
       <c r="C12" s="8" t="s">
         <v>47</v>
       </c>
@@ -1034,257 +1056,264 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="5"/>
+    <row r="13" spans="3:7">
+      <c r="C13" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="D13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14" s="15" t="s">
+    <row r="14" spans="3:7">
+      <c r="C14" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" s="15" t="s">
+      <c r="E14" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15" s="11"/>
+      <c r="D15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="19"/>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="14"/>
-      <c r="D16" s="15" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="3:7">
+      <c r="C16" s="11"/>
+      <c r="D16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="19"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="14"/>
-      <c r="D17" s="15" t="s">
+      <c r="E16" s="12"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17" s="11"/>
+      <c r="D17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="14"/>
-      <c r="D18" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="19"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="14"/>
-      <c r="D19" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="19"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18" s="11"/>
+      <c r="D18" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="11"/>
+      <c r="D19" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="3:6">
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6">
       <c r="C21" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="14" t="s">
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="16"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="14" t="s">
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="14" t="s">
+      <c r="F23" s="15"/>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="16"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="14" t="s">
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="14" t="s">
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="16"/>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="14" t="s">
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="C27" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="14" t="s">
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="16"/>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="14" t="s">
+      <c r="F28" s="15"/>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="16"/>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="14"/>
-      <c r="D30" s="15" t="s">
+      <c r="F29" s="15"/>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30" s="11"/>
+      <c r="D30" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="16"/>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="14"/>
-      <c r="D31" s="15" t="s">
+      <c r="F30" s="15"/>
+    </row>
+    <row r="31" spans="3:6">
+      <c r="C31" s="11"/>
+      <c r="D31" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="16"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="14"/>
-      <c r="D32" s="15" t="s">
+      <c r="F31" s="15"/>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" s="11"/>
+      <c r="D32" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="16"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="14"/>
-      <c r="D33" s="15" t="s">
+      <c r="F32" s="15"/>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="11"/>
+      <c r="D33" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C34" s="14"/>
-      <c r="D34" s="15" t="s">
+      <c r="F33" s="15"/>
+    </row>
+    <row r="34" spans="3:7">
+      <c r="C34" s="11"/>
+      <c r="D34" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="16"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C35" s="14" t="s">
+      <c r="F34" s="15"/>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="C35" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="16"/>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="15"/>
+    </row>
+    <row r="36" spans="3:7">
       <c r="C36" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="19"/>
+    </row>
+    <row r="37" spans="3:7">
       <c r="C37" s="5" t="s">
         <v>58</v>
       </c>
@@ -1298,415 +1327,405 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C38" s="14" t="s">
+    <row r="38" spans="3:7">
+      <c r="C38" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C39" s="14" t="s">
+    <row r="39" spans="3:7">
+      <c r="C39" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="E39" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" s="15"/>
+    </row>
+    <row r="40" spans="3:7">
+      <c r="C40" s="11"/>
+      <c r="D40" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E40" s="12"/>
+      <c r="F40" s="13"/>
+    </row>
+    <row r="41" spans="3:7">
+      <c r="C41" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7">
+      <c r="C42" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C40" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E40" s="15" t="s">
+      <c r="F42" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7">
+      <c r="C43" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F43" s="15"/>
+    </row>
+    <row r="44" spans="3:7">
+      <c r="C44" s="11"/>
+      <c r="D44" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="C45" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="15"/>
+    </row>
+    <row r="46" spans="3:7">
+      <c r="C46" s="11"/>
+      <c r="D46" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="3:7">
+      <c r="C47" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47" s="13"/>
+      <c r="G47" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7">
+      <c r="C48" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F48" s="13"/>
+      <c r="G48" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6">
+      <c r="C49" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F49" s="21"/>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="C50" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6">
+      <c r="C51" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51" s="15"/>
+    </row>
+    <row r="52" spans="3:6">
+      <c r="C52" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6">
+      <c r="C53" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F53" s="15"/>
+    </row>
+    <row r="54" spans="3:6">
+      <c r="C54" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6">
+      <c r="C55" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" s="15"/>
+    </row>
+    <row r="56" spans="3:6">
+      <c r="C56" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6">
+      <c r="C57" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="3:6">
+      <c r="C58" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6">
+      <c r="C59" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F59" s="15"/>
+    </row>
+    <row r="60" spans="3:6">
+      <c r="C60" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6">
+      <c r="C61" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F61" s="13"/>
+    </row>
+    <row r="62" spans="3:6">
+      <c r="C62" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F62" s="13"/>
+    </row>
+    <row r="63" spans="3:6">
+      <c r="C63" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C41" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" s="15" t="s">
+      <c r="F63" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6">
+      <c r="C64" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6">
+      <c r="C65" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" s="15"/>
+    </row>
+    <row r="66" spans="3:6">
+      <c r="C66" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F66" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C42" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E42" s="15" t="s">
+    <row r="67" spans="3:6">
+      <c r="C67" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="19" t="s">
+      <c r="F67" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C43" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C44" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="15" t="s">
+    <row r="68" spans="3:6">
+      <c r="C68" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F68" s="19"/>
+    </row>
+    <row r="72" spans="3:6">
+      <c r="F72" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C45" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F45" s="16"/>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C46" s="14"/>
-      <c r="D46" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="19"/>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C47" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F47" s="19"/>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C48" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F48" s="19"/>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C49" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="19"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C50" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C51" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="19"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C52" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C53" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="19"/>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C54" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F54" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C55" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="19"/>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C56" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C57" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E57" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="19"/>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C58" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C59" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D59" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="19"/>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C60" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F60" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C61" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F61" s="19"/>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C62" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F62" s="19"/>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C63" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C64" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D64" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C65" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F65" s="16"/>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C66" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C67" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C68" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E68" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="F68" s="18"/>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="F72" s="1" t="s">
-        <v>77</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="27">
     <mergeCell ref="E68:F68"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
@@ -1714,11 +1733,14 @@
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E59:F59"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
@@ -1726,6 +1748,11 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1733,24 +1760,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Increment, Decrement, Compare & Test added.
</commit_message>
<xml_diff>
--- a/opcodes-fic.xlsx
+++ b/opcodes-fic.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\faculta\an3\FIC\FIC_proiect\0xcHa0s\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A8B77-73A6-4422-BB9D-5049983DBB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="139">
   <si>
     <t>Opcode</t>
   </si>
@@ -436,13 +430,16 @@
   </si>
   <si>
     <t>Roxi</t>
+  </si>
+  <si>
+    <t>Tudor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,8 +447,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,6 +480,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -600,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -613,16 +629,27 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -631,18 +658,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,7 +683,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -703,7 +725,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -735,27 +757,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -787,24 +791,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -980,14 +966,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="10.44140625" style="1" customWidth="1"/>
@@ -998,31 +984,34 @@
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="16" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="15" t="s">
         <v>137</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
+      <c r="A3" s="25" t="s">
+        <v>138</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="20" t="s">
+    <row r="5" spans="1:7">
+      <c r="C5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1035,8 +1024,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="20" t="s">
+    <row r="6" spans="1:7">
+      <c r="C6" s="12" t="s">
         <v>108</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1047,7 +1036,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1061,7 +1050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="C9" s="4" t="s">
         <v>54</v>
       </c>
@@ -1089,7 +1078,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="C10" s="7" t="s">
         <v>55</v>
       </c>
@@ -1103,8 +1092,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="21" t="s">
+    <row r="11" spans="1:7">
+      <c r="C11" s="27" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1117,8 +1106,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="22" t="s">
+    <row r="12" spans="1:7">
+      <c r="C12" s="28" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1131,8 +1120,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="23" t="s">
+    <row r="13" spans="1:7">
+      <c r="C13" s="14" t="s">
         <v>106</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1143,8 +1132,8 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="23" t="s">
+    <row r="14" spans="1:7">
+      <c r="C14" s="14" t="s">
         <v>107</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1158,42 +1147,42 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="C15" s="10"/>
       <c r="D15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="C16" s="10"/>
       <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6">
       <c r="C17" s="10"/>
       <c r="D17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6">
       <c r="C18" s="10"/>
       <c r="D18" s="1" t="s">
         <v>103</v>
       </c>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6">
       <c r="C19" s="10"/>
       <c r="D19" s="1" t="s">
         <v>104</v>
       </c>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6">
       <c r="C20" s="7"/>
       <c r="D20" s="8" t="s">
         <v>105</v>
@@ -1201,190 +1190,190 @@
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6">
       <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="19"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="3:6">
       <c r="C22" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="3:6">
       <c r="C23" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="15"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="3:6">
       <c r="C24" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="3:6">
       <c r="C25" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="3:6">
       <c r="C26" s="10" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="3:6">
       <c r="C27" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="15"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="3:6">
       <c r="C28" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="15"/>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="3:6">
       <c r="C29" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="15"/>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="3:6">
       <c r="C30" s="10"/>
       <c r="D30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="15"/>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="3:6">
       <c r="C31" s="10"/>
       <c r="D31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="3:6">
       <c r="C32" s="10"/>
       <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="15"/>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="3:7">
       <c r="C33" s="10"/>
       <c r="D33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="15"/>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="3:7">
       <c r="C34" s="10"/>
       <c r="D34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="15"/>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="3:7">
       <c r="C35" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="15"/>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="3:7">
       <c r="C36" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="13"/>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C37" s="21" t="s">
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="C37" s="13" t="s">
         <v>58</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -1397,8 +1386,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C38" s="23" t="s">
+    <row r="38" spans="3:7">
+      <c r="C38" s="14" t="s">
         <v>59</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1411,27 +1400,27 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C39" s="23" t="s">
+    <row r="39" spans="3:7">
+      <c r="C39" s="14" t="s">
         <v>127</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F39" s="15"/>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="3:7">
       <c r="C40" s="10"/>
       <c r="D40" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F40" s="11"/>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C41" s="23" t="s">
+    <row r="41" spans="3:7">
+      <c r="C41" s="14" t="s">
         <v>63</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -1444,8 +1433,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C42" s="23" t="s">
+    <row r="42" spans="3:7">
+      <c r="C42" s="14" t="s">
         <v>64</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1458,46 +1447,46 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C43" s="23" t="s">
+    <row r="43" spans="3:7">
+      <c r="C43" s="14" t="s">
         <v>129</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F43" s="15"/>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="3:7">
       <c r="C44" s="10"/>
       <c r="D44" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F44" s="11"/>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:7">
       <c r="C45" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F45" s="15"/>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="3:7">
       <c r="C46" s="10"/>
       <c r="D46" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F46" s="11"/>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C47" s="10" t="s">
+    <row r="47" spans="3:7">
+      <c r="C47" s="26" t="s">
         <v>88</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1511,8 +1500,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C48" s="10" t="s">
+    <row r="48" spans="3:7">
+      <c r="C48" s="26" t="s">
         <v>90</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1526,20 +1515,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C49" s="23" t="s">
+    <row r="49" spans="3:6">
+      <c r="C49" s="14" t="s">
         <v>130</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="E49" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="F49" s="17"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C50" s="23" t="s">
+      <c r="F49" s="24"/>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="C50" s="14" t="s">
         <v>111</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1552,20 +1541,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C51" s="23" t="s">
+    <row r="51" spans="3:6">
+      <c r="C51" s="14" t="s">
         <v>131</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F51" s="15"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C52" s="23" t="s">
+      <c r="F51" s="18"/>
+    </row>
+    <row r="52" spans="3:6">
+      <c r="C52" s="14" t="s">
         <v>112</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -1578,20 +1567,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C53" s="23" t="s">
+    <row r="53" spans="3:6">
+      <c r="C53" s="14" t="s">
         <v>133</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F53" s="15"/>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C54" s="23" t="s">
+      <c r="F53" s="18"/>
+    </row>
+    <row r="54" spans="3:6">
+      <c r="C54" s="14" t="s">
         <v>113</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -1604,20 +1593,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C55" s="23" t="s">
+    <row r="55" spans="3:6">
+      <c r="C55" s="14" t="s">
         <v>132</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F55" s="15"/>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C56" s="23" t="s">
+      <c r="F55" s="18"/>
+    </row>
+    <row r="56" spans="3:6">
+      <c r="C56" s="14" t="s">
         <v>118</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -1630,20 +1619,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C57" s="23" t="s">
+    <row r="57" spans="3:6">
+      <c r="C57" s="14" t="s">
         <v>134</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="14" t="s">
+      <c r="E57" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F57" s="15"/>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C58" s="23" t="s">
+      <c r="F57" s="18"/>
+    </row>
+    <row r="58" spans="3:6">
+      <c r="C58" s="14" t="s">
         <v>119</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -1656,20 +1645,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C59" s="23" t="s">
+    <row r="59" spans="3:6">
+      <c r="C59" s="14" t="s">
         <v>135</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="E59" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F59" s="15"/>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C60" s="23" t="s">
+      <c r="F59" s="18"/>
+    </row>
+    <row r="60" spans="3:6">
+      <c r="C60" s="14" t="s">
         <v>120</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -1682,8 +1671,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C61" s="23" t="s">
+    <row r="61" spans="3:6">
+      <c r="C61" s="14" t="s">
         <v>85</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -1694,8 +1683,8 @@
       </c>
       <c r="F61" s="11"/>
     </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C62" s="23" t="s">
+    <row r="62" spans="3:6">
+      <c r="C62" s="14" t="s">
         <v>92</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -1706,8 +1695,8 @@
       </c>
       <c r="F62" s="11"/>
     </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C63" s="10" t="s">
+    <row r="63" spans="3:6">
+      <c r="C63" s="29" t="s">
         <v>114</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -1720,8 +1709,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C64" s="10" t="s">
+    <row r="64" spans="3:6">
+      <c r="C64" s="29" t="s">
         <v>101</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -1734,20 +1723,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C65" s="10" t="s">
+    <row r="65" spans="3:6">
+      <c r="C65" s="29" t="s">
         <v>115</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F65" s="15"/>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C66" s="10" t="s">
+      <c r="F65" s="18"/>
+    </row>
+    <row r="66" spans="3:6">
+      <c r="C66" s="30" t="s">
         <v>116</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -1760,8 +1749,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C67" s="10" t="s">
+    <row r="67" spans="3:6">
+      <c r="C67" s="30" t="s">
         <v>102</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -1774,37 +1763,25 @@
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C68" s="7" t="s">
+    <row r="68" spans="3:6">
+      <c r="C68" s="31" t="s">
         <v>117</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F68" s="13"/>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F68" s="22"/>
+    </row>
+    <row r="72" spans="3:6">
       <c r="F72" s="1" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
     <mergeCell ref="E68:F68"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
@@ -1820,6 +1797,18 @@
     <mergeCell ref="E53:F53"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1827,24 +1816,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed label use before declaration
</commit_message>
<xml_diff>
--- a/opcodes-fic.xlsx
+++ b/opcodes-fic.xlsx
@@ -649,16 +649,26 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -667,16 +677,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,7 +1022,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="25" t="s">
         <v>139</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1056,7 +1056,7 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1070,7 +1070,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="24" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1084,7 +1084,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1098,7 +1098,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="24" t="s">
         <v>55</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -1210,7 +1210,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="23" t="s">
         <v>33</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -1222,174 +1222,174 @@
       <c r="F21" s="30"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="26" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="28"/>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="26" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="26"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="26" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="26"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="26" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="26"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="26" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="26"/>
+      <c r="F26" s="28"/>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="26"/>
+      <c r="F27" s="28"/>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="26" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="26"/>
+      <c r="F28" s="28"/>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="26" t="s">
         <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="26"/>
+      <c r="F29" s="28"/>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="34"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="28"/>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="34"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="34"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="26"/>
+      <c r="F32" s="28"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C33" s="34"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="26"/>
+      <c r="F33" s="28"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C34" s="34"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="26"/>
+      <c r="F34" s="28"/>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="26" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E35" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="26"/>
+      <c r="F35" s="28"/>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="24" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="24"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C37" s="12" t="s">
@@ -1426,10 +1426,10 @@
       <c r="D39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="25" t="s">
+      <c r="E39" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="28"/>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C40" s="9"/>
@@ -1473,10 +1473,10 @@
       <c r="D43" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="25" t="s">
+      <c r="E43" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="F43" s="26"/>
+      <c r="F43" s="28"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C44" s="9"/>
@@ -1486,16 +1486,16 @@
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="26" t="s">
         <v>69</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="25" t="s">
+      <c r="E45" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F45" s="26"/>
+      <c r="F45" s="28"/>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C46" s="9"/>
@@ -1541,10 +1541,10 @@
       <c r="D49" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E49" s="27" t="s">
+      <c r="E49" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="F49" s="28"/>
+      <c r="F49" s="34"/>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C50" s="13" t="s">
@@ -1567,10 +1567,10 @@
       <c r="D51" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="25" t="s">
+      <c r="E51" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="F51" s="26"/>
+      <c r="F51" s="28"/>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C52" s="13" t="s">
@@ -1593,10 +1593,10 @@
       <c r="D53" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="25" t="s">
+      <c r="E53" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="F53" s="26"/>
+      <c r="F53" s="28"/>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C54" s="13" t="s">
@@ -1619,10 +1619,10 @@
       <c r="D55" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E55" s="25" t="s">
+      <c r="E55" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="F55" s="26"/>
+      <c r="F55" s="28"/>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C56" s="13" t="s">
@@ -1645,10 +1645,10 @@
       <c r="D57" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="25" t="s">
+      <c r="E57" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="F57" s="26"/>
+      <c r="F57" s="28"/>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C58" s="13" t="s">
@@ -1671,10 +1671,10 @@
       <c r="D59" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E59" s="25" t="s">
+      <c r="E59" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="F59" s="26"/>
+      <c r="F59" s="28"/>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C60" s="13" t="s">
@@ -1749,10 +1749,10 @@
       <c r="D65" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E65" s="25" t="s">
+      <c r="E65" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="F65" s="26"/>
+      <c r="F65" s="28"/>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C66" s="21" t="s">
@@ -1789,10 +1789,10 @@
       <c r="D68" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E68" s="23" t="s">
+      <c r="E68" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="F68" s="24"/>
+      <c r="F68" s="32"/>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.3">
       <c r="F72" s="1" t="s">
@@ -1801,18 +1801,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
     <mergeCell ref="E68:F68"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
@@ -1828,6 +1816,18 @@
     <mergeCell ref="E53:F53"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>